<commit_message>
Added tests to Selenium test plan for Green Kart practice website.
</commit_message>
<xml_diff>
--- a/TestCaseOutline.xlsx
+++ b/TestCaseOutline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Workspaces\TestingPorfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C887D39-E804-462B-A53C-034E37AF156A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF28191A-F18F-4FA9-A0D2-76B950DFAC0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
+    <workbookView xWindow="38280" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -49,6 +49,144 @@
   </si>
   <si>
     <t>App</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>https://rahulshettyacademy.com/seleniumPractise/#/</t>
+  </si>
+  <si>
+    <t>https://rahulshettyacademy.com/AutomationPractice/</t>
+  </si>
+  <si>
+    <t>https://rahulshettyacademy.com/angularpractice/</t>
+  </si>
+  <si>
+    <t>Green Kart - Shopping Page</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Product to search for.</t>
+  </si>
+  <si>
+    <t>Verify the company logo is displayed in header when navigating to page.</t>
+  </si>
+  <si>
+    <t>Partial string to search for.</t>
+  </si>
+  <si>
+    <t>Invalid string to search for.</t>
+  </si>
+  <si>
+    <t>Verify product list returns all products after search has been cleared.</t>
+  </si>
+  <si>
+    <t>Product list</t>
+  </si>
+  <si>
+    <t>Verify product list shows the correct price for each item.</t>
+  </si>
+  <si>
+    <t>Verify product list shows the expected products when using a full product search.</t>
+  </si>
+  <si>
+    <t>Verify product list shows products when using a parital product search.</t>
+  </si>
+  <si>
+    <t>Verify product list shows the expected error when using an invalid product search.</t>
+  </si>
+  <si>
+    <t>Product list with prices</t>
+  </si>
+  <si>
+    <t>Verify limited offer link navigates to the correct page.</t>
+  </si>
+  <si>
+    <t>Verify Top Deals link navigates to the correct page.</t>
+  </si>
+  <si>
+    <t>Verify Flight Booking link navigates to the correct page.</t>
+  </si>
+  <si>
+    <t>Verify Proceed to Checkout button in the cart is disabled when cart is empty.</t>
+  </si>
+  <si>
+    <t>Verify cart shows the cart is empty message when cart is empty.</t>
+  </si>
+  <si>
+    <t>https://rahulshettyacademy.com/dropdownsPractise/</t>
+  </si>
+  <si>
+    <t>Verify product shows the added message when it is added to the cart.</t>
+  </si>
+  <si>
+    <t>Verify cart shows product when a product has been added to the cart.</t>
+  </si>
+  <si>
+    <t>Verify cart shows the correct quantity if multiple of one item are added to the cart.</t>
+  </si>
+  <si>
+    <t>Verify cart shows all items in cart when multiple different items have been added.</t>
+  </si>
+  <si>
+    <t>Verify product list shows products in the correct order.</t>
+  </si>
+  <si>
+    <t>Verify cart no longer shows items that have been deleted from the cart.</t>
+  </si>
+  <si>
+    <t>Verify cart shows the correct total for items that have been added to the cart.</t>
+  </si>
+  <si>
+    <t>Green Kart - Checkout Page</t>
+  </si>
+  <si>
+    <t>Verify table lists all products that were added to the cart.</t>
+  </si>
+  <si>
+    <t>Verify cart still shows added items after refreshing the page.</t>
+  </si>
+  <si>
+    <t>Verify table has the correct price for each product that was added to the cart.</t>
+  </si>
+  <si>
+    <t>Verify table has the correct quantity for each product that was added to the cart.</t>
+  </si>
+  <si>
+    <t>Veirfy table is calculating the total correctly for each product added to the cart.</t>
+  </si>
+  <si>
+    <t>Verify total is displayed and correct for all items in the cart.</t>
+  </si>
+  <si>
+    <t>Verify coupon code shows correct error message when an invalid code is entered.</t>
+  </si>
+  <si>
+    <t>Verify coupon code shows correct success message when a valid code is entered.</t>
+  </si>
+  <si>
+    <t>Verify total after discount is calculated and displayed correctly when entering a valid coupon.</t>
+  </si>
+  <si>
+    <t>Verify place order button takes user to the shipping page.</t>
+  </si>
+  <si>
+    <t>Green Kart - Shipping Page</t>
+  </si>
+  <si>
+    <t>Verify country dropdown allows a country to be selected.</t>
+  </si>
+  <si>
+    <t>Verify error message is displayed if terms and conditions are not agreed to.</t>
+  </si>
+  <si>
+    <t>Verify success message is displayed upon successfully placing order.</t>
+  </si>
+  <si>
+    <t>Verify shopping page is shown after completing a successful order.</t>
   </si>
 </sst>
 </file>
@@ -400,22 +538,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01736B7F-A2A0-4AAD-A91F-D8A3A1F0F951}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="7" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -436,6 +576,397 @@
       </c>
       <c r="G1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added preconditions and expected results to Green Kart Selenium test cases.
</commit_message>
<xml_diff>
--- a/TestCaseOutline.xlsx
+++ b/TestCaseOutline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Workspaces\TestingPorfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF28191A-F18F-4FA9-A0D2-76B950DFAC0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0912471-CCE8-45F7-A2B0-77AF1F61BDCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Green Kart - Shopping Page</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Product to search for.</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Verify table has the correct quantity for each product that was added to the cart.</t>
   </si>
   <si>
-    <t>Veirfy table is calculating the total correctly for each product added to the cart.</t>
-  </si>
-  <si>
     <t>Verify total is displayed and correct for all items in the cart.</t>
   </si>
   <si>
@@ -187,16 +181,142 @@
   </si>
   <si>
     <t>Verify shopping page is shown after completing a successful order.</t>
+  </si>
+  <si>
+    <t>Verify product quantity can be changed using the increase and decrease buttons.</t>
+  </si>
+  <si>
+    <t>Product list, and expected order.</t>
+  </si>
+  <si>
+    <t>Verify table is calculating the total correctly for each product added to the cart.</t>
+  </si>
+  <si>
+    <t>valid coupon code</t>
+  </si>
+  <si>
+    <t>A product search entered.</t>
+  </si>
+  <si>
+    <t>Products added to cart</t>
+  </si>
+  <si>
+    <t>Company logo is visible and located in header.</t>
+  </si>
+  <si>
+    <t>Only the product that was entered in the search bar is present.</t>
+  </si>
+  <si>
+    <t>Only products that contain the sub string that was searched for are present.</t>
+  </si>
+  <si>
+    <t>"Sorry, no products matched your search!" is displayed in the product list.</t>
+  </si>
+  <si>
+    <t>All products are visible again.</t>
+  </si>
+  <si>
+    <t>The price of each product is displayed correctly.</t>
+  </si>
+  <si>
+    <t>The product list shows the products in the specified order.</t>
+  </si>
+  <si>
+    <t>Clicking "Top Deals" takes the user to "https://rahulshettyacademy.com/seleniumPractise/#/offers".</t>
+  </si>
+  <si>
+    <t>Clicking "Flight Booking"  takes the user to "https://rahulshettyacademy.com/seleniumPractise/#/offers".</t>
+  </si>
+  <si>
+    <t>Clicking "Free Access to InterviewQues/ResumeAssistance/Material" takes user to "https://rahulshettyacademy.com/#/documents-request"</t>
+  </si>
+  <si>
+    <t>Proceed to checkout button has class "disabled" and is not clickable.</t>
+  </si>
+  <si>
+    <t>"You cart is empty" is displayed in the cart.</t>
+  </si>
+  <si>
+    <t>"ADDED" is shown in the "ADD TO CART" button after clicking the button.</t>
+  </si>
+  <si>
+    <t>Product quantity increases/decreases upon clicking the plus/minus buttons on a product tile.</t>
+  </si>
+  <si>
+    <t>Cart includes a product after the "ADD TO CART" button has been clicked.</t>
+  </si>
+  <si>
+    <t>Cart shows all items that were added to the cart.</t>
+  </si>
+  <si>
+    <t>Cart shows the correct quantity of an item after it has been added to the cart.</t>
+  </si>
+  <si>
+    <t>Cart persists all products after refreshing the page.</t>
+  </si>
+  <si>
+    <t>Product is no longer in the cart.</t>
+  </si>
+  <si>
+    <t>Total of all items is correct in the cart.</t>
+  </si>
+  <si>
+    <t>All products that were added to cart are visible.</t>
+  </si>
+  <si>
+    <t>The correct quantity for each product that was added is correct.</t>
+  </si>
+  <si>
+    <t>The price of each product that was added is correct.</t>
+  </si>
+  <si>
+    <t>The total for each product is being correctly calculated based on price and quantity.</t>
+  </si>
+  <si>
+    <t>The total for all items is correctly being displayed below the table.</t>
+  </si>
+  <si>
+    <t>"Invalid code ..!" is shown after entering a coupon code.</t>
+  </si>
+  <si>
+    <t>"No Idea" is shown after entering a coupon code.</t>
+  </si>
+  <si>
+    <t>Total is calculated correctly based on discount percentage.</t>
+  </si>
+  <si>
+    <t>User is taken to "https://rahulshettyacademy.com/seleniumPractise/#/country" upon clicking the button.</t>
+  </si>
+  <si>
+    <t>A country is able to be selected from the drop down list.</t>
+  </si>
+  <si>
+    <t>"Please accept Terms &amp; Conditions - Required" is displayed.</t>
+  </si>
+  <si>
+    <t>"Thank you, your order has been placed successfully
+You'll be redirected to Home page shortly!!" is displayed.</t>
+  </si>
+  <si>
+    <t>User is redirected to "https://rahulshettyacademy.com/seleniumPractise/#/".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,13 +339,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,10 +664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01736B7F-A2A0-4AAD-A91F-D8A3A1F0F951}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,10 +676,10 @@
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="91.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="52.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -574,28 +701,8 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -603,64 +710,79 @@
         <v>11</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="G6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -668,13 +790,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -682,71 +810,89 @@
         <v>11</v>
       </c>
       <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="G11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -754,222 +900,355 @@
         <v>11</v>
       </c>
       <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="G17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="G18" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
+      <c r="G19" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
       <c r="C20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="E33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" location="/" xr:uid="{AAB5D607-33E5-4411-A2DE-CF59E7690327}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>